<commit_message>
updated resource recovery code for system simulation
</commit_message>
<xml_diff>
--- a/dmsan/reclaimer/scores/China/parameters.xlsx
+++ b/dmsan/reclaimer/scores/China/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reclaimer B" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reclaimer C" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Reclaimer B" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Reclaimer C" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H282"/>
+  <dimension ref="A1:H314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>('Ion exchange reclaimer-B6', 'TN removal [% removal ]')</t>
+          <t>('Ion exchange reclaimer-B6', 'TN removal [ratio]')</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>('Ion exchange reclaimer-B6', 'Desorption recovery efficiency [% recovery]')</t>
+          <t>('Ion exchange reclaimer-B6', 'Desorption recovery efficiency [ratio]')</t>
         </is>
       </c>
       <c r="C163" t="inlineStr"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>('LCA', 'CH4 resources CF [points/kg CH4]')</t>
+          <t>('LCA', 'N2O CF [kg CO2-eq/kg N2O]')</t>
         </is>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O CF [kg CO2-eq/kg N2O]')</t>
+          <t>('LCA', 'N2O ecosystems CF [points/kg N2O]')</t>
         </is>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O ecosystems CF [points/kg N2O]')</t>
+          <t>('LCA', 'N2O health CF [points/kg N2O]')</t>
         </is>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O health CF [points/kg N2O]')</t>
+          <t>('LCA', 'N fertilizer CF [kg CO2-eq/kg N]')</t>
         </is>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O resources CF [points/kg N2O]')</t>
+          <t>('LCA', 'N fertilizer ecosystems CF [points/kg N]')</t>
         </is>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-Global warming [kg CO2-eq/m3]')</t>
+          <t>('LCA', 'N fertilizer health CF [points/kg N]')</t>
         </is>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'N fertilizer resources CF [points/kg N]')</t>
         </is>
       </c>
       <c r="C188" t="inlineStr"/>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'P fertilizer CF [kg CO2-eq/kg P]')</t>
         </is>
       </c>
       <c r="C189" t="inlineStr"/>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-Global warming [kg CO2-eq/m3]')</t>
+          <t>('LCA', 'P fertilizer ecosystems CF [points/kg P]')</t>
         </is>
       </c>
       <c r="C190" t="inlineStr"/>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'P fertilizer health CF [points/kg P]')</t>
         </is>
       </c>
       <c r="C191" t="inlineStr"/>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'P fertilizer resources CF [points/kg P]')</t>
         </is>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'K fertilizer CF [kg CO2-eq/kg K]')</t>
         </is>
       </c>
       <c r="C193" t="inlineStr"/>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Conc nh3 CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Conc nh3 ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Conc nh3 health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-Global warming [kg CO2-eq/m3]')</t>
+          <t>('LCA', 'Conc nh3 resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-Global warming [kg CO2-eq/tonne*km]')</t>
+          <t>('LCA', 'GAC CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'GAC ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C199" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-Global warming [kg CO2-eq/ea]')</t>
+          <t>('LCA', 'GAC health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-Global warming [kg CO2-eq/m2]')</t>
+          <t>('LCA', 'GAC resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C207" t="inlineStr"/>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C208" t="inlineStr"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-H ecosystems [points/m3]')</t>
+          <t>('LCA', 'Mg oh2 CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Mg oh2 ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Mg oh2 health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -3853,7 +3853,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-H ecosystems [points/m3]')</t>
+          <t>('LCA', 'Mg oh2 resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Excavation-Global warming [kg CO2-eq/m3]')</t>
         </is>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Brick-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Cement-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C216" t="inlineStr"/>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-h ecosystems [points/kg]')</t>
+          <t>('LCA', 'Concrete-Global warming [kg CO2-eq/m3]')</t>
         </is>
       </c>
       <c r="C217" t="inlineStr"/>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-h ecosystems [points/kg]')</t>
+          <t>('LCA', 'Gravel-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Plastic-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-H ecosystems [points/m3]')</t>
+          <t>('LCA', 'Sand-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-H ecosystems [points/tonne*km]')</t>
+          <t>('LCA', 'Stainless steel-global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet-global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-H ecosystems [points/ea]')</t>
+          <t>('LCA', 'Steel-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-H ecosystems [points/m2]')</t>
+          <t>('LCA', 'Wood-Global warming [kg CO2-eq/m3]')</t>
         </is>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Trucking-Global warming [kg CO2-eq/tonne*km]')</t>
         </is>
       </c>
       <c r="C225" t="inlineStr"/>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Metal-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C226" t="inlineStr"/>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Pump-Global warming [kg CO2-eq/ea]')</t>
         </is>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Solar-Global warming [kg CO2-eq/m2]')</t>
         </is>
       </c>
       <c r="C228" t="inlineStr"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-h ecosystems [points/kg]')</t>
+          <t>('LCA', 'Fan-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C229" t="inlineStr"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Battery-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C230" t="inlineStr"/>
@@ -4141,7 +4141,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Ceramic-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C231" t="inlineStr"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'FRP-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C232" t="inlineStr"/>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-H health [points/m3]')</t>
+          <t>('LCA', 'Na cl-global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C233" t="inlineStr"/>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-H health [points/kg]')</t>
+          <t>('LCA', 'Motor-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C234" t="inlineStr"/>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-H health [points/kg]')</t>
+          <t>('LCA', 'Titanium-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C235" t="inlineStr"/>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-H health [points/m3]')</t>
+          <t>('LCA', 'PVC-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C236" t="inlineStr"/>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-H health [points/kg]')</t>
+          <t>('LCA', 'Excavation-H ecosystems [points/m3]')</t>
         </is>
       </c>
       <c r="C237" t="inlineStr"/>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-H health [points/kg]')</t>
+          <t>('LCA', 'Brick-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C238" t="inlineStr"/>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-H health [points/kg]')</t>
+          <t>('LCA', 'Cement-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C239" t="inlineStr"/>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-h health [points/kg]')</t>
+          <t>('LCA', 'Concrete-H ecosystems [points/m3]')</t>
         </is>
       </c>
       <c r="C240" t="inlineStr"/>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-h health [points/kg]')</t>
+          <t>('LCA', 'Gravel-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C241" t="inlineStr"/>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-H health [points/kg]')</t>
+          <t>('LCA', 'Plastic-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C242" t="inlineStr"/>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-H health [points/m3]')</t>
+          <t>('LCA', 'Sand-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C243" t="inlineStr"/>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-H health [points/tonne*km]')</t>
+          <t>('LCA', 'Stainless steel-h ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C244" t="inlineStr"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-H health [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet-h ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C245" t="inlineStr"/>
@@ -4381,7 +4381,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-H health [points/ea]')</t>
+          <t>('LCA', 'Steel-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C246" t="inlineStr"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-H health [points/m2]')</t>
+          <t>('LCA', 'Wood-H ecosystems [points/m3]')</t>
         </is>
       </c>
       <c r="C247" t="inlineStr"/>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-H health [points/kg]')</t>
+          <t>('LCA', 'Trucking-H ecosystems [points/tonne*km]')</t>
         </is>
       </c>
       <c r="C248" t="inlineStr"/>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-H health [points/kg]')</t>
+          <t>('LCA', 'Metal-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C249" t="inlineStr"/>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-H health [points/kg]')</t>
+          <t>('LCA', 'Pump-H ecosystems [points/ea]')</t>
         </is>
       </c>
       <c r="C250" t="inlineStr"/>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-H health [points/kg]')</t>
+          <t>('LCA', 'Solar-H ecosystems [points/m2]')</t>
         </is>
       </c>
       <c r="C251" t="inlineStr"/>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-h health [points/kg]')</t>
+          <t>('LCA', 'Fan-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C252" t="inlineStr"/>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-H health [points/kg]')</t>
+          <t>('LCA', 'Battery-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C253" t="inlineStr"/>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-H health [points/kg]')</t>
+          <t>('LCA', 'Ceramic-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C254" t="inlineStr"/>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-H health [points/kg]')</t>
+          <t>('LCA', 'FRP-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C255" t="inlineStr"/>
@@ -4541,7 +4541,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-H resources [points/m3]')</t>
+          <t>('LCA', 'Na cl-h ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C256" t="inlineStr"/>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-H resources [points/kg]')</t>
+          <t>('LCA', 'Motor-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C257" t="inlineStr"/>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-H resources [points/kg]')</t>
+          <t>('LCA', 'Titanium-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C258" t="inlineStr"/>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-H resources [points/m3]')</t>
+          <t>('LCA', 'PVC-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C259" t="inlineStr"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-H resources [points/kg]')</t>
+          <t>('LCA', 'Excavation-H health [points/m3]')</t>
         </is>
       </c>
       <c r="C260" t="inlineStr"/>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-H resources [points/kg]')</t>
+          <t>('LCA', 'Brick-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C261" t="inlineStr"/>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-H resources [points/kg]')</t>
+          <t>('LCA', 'Cement-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C262" t="inlineStr"/>
@@ -4653,7 +4653,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-h resources [points/kg]')</t>
+          <t>('LCA', 'Concrete-H health [points/m3]')</t>
         </is>
       </c>
       <c r="C263" t="inlineStr"/>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-h resources [points/kg]')</t>
+          <t>('LCA', 'Gravel-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C264" t="inlineStr"/>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-H resources [points/kg]')</t>
+          <t>('LCA', 'Plastic-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C265" t="inlineStr"/>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-H resources [points/m3]')</t>
+          <t>('LCA', 'Sand-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C266" t="inlineStr"/>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-H resources [points/tonne*km]')</t>
+          <t>('LCA', 'Stainless steel-h health [points/kg]')</t>
         </is>
       </c>
       <c r="C267" t="inlineStr"/>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-H resources [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet-h health [points/kg]')</t>
         </is>
       </c>
       <c r="C268" t="inlineStr"/>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-H resources [points/ea]')</t>
+          <t>('LCA', 'Steel-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C269" t="inlineStr"/>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-H resources [points/m2]')</t>
+          <t>('LCA', 'Wood-H health [points/m3]')</t>
         </is>
       </c>
       <c r="C270" t="inlineStr"/>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-H resources [points/kg]')</t>
+          <t>('LCA', 'Trucking-H health [points/tonne*km]')</t>
         </is>
       </c>
       <c r="C271" t="inlineStr"/>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-H resources [points/kg]')</t>
+          <t>('LCA', 'Metal-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C272" t="inlineStr"/>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-H resources [points/kg]')</t>
+          <t>('LCA', 'Pump-H health [points/ea]')</t>
         </is>
       </c>
       <c r="C273" t="inlineStr"/>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-H resources [points/kg]')</t>
+          <t>('LCA', 'Solar-H health [points/m2]')</t>
         </is>
       </c>
       <c r="C274" t="inlineStr"/>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-h resources [points/kg]')</t>
+          <t>('LCA', 'Fan-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C275" t="inlineStr"/>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-H resources [points/kg]')</t>
+          <t>('LCA', 'Battery-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C276" t="inlineStr"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-H resources [points/kg]')</t>
+          <t>('LCA', 'Ceramic-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C277" t="inlineStr"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-H resources [points/kg]')</t>
+          <t>('LCA', 'FRP-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C278" t="inlineStr"/>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity CF [kg CO2-eq/kWh]')</t>
+          <t>('LCA', 'Na cl-h health [points/kg]')</t>
         </is>
       </c>
       <c r="C279" t="inlineStr"/>
@@ -4925,7 +4925,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity ecosystems CF [points/kWh]')</t>
+          <t>('LCA', 'Motor-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C280" t="inlineStr"/>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity health CF [points/kWh]')</t>
+          <t>('LCA', 'Titanium-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C281" t="inlineStr"/>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity resources CF [points/kWh]')</t>
+          <t>('LCA', 'PVC-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C282" t="inlineStr"/>
@@ -4966,6 +4966,518 @@
       <c r="F282" t="inlineStr"/>
       <c r="G282" t="inlineStr"/>
       <c r="H282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>('LCA', 'Excavation-H resources [points/m3]')</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr"/>
+      <c r="D283" t="inlineStr"/>
+      <c r="E283" t="inlineStr"/>
+      <c r="F283" t="inlineStr"/>
+      <c r="G283" t="inlineStr"/>
+      <c r="H283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>('LCA', 'Brick-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr"/>
+      <c r="D284" t="inlineStr"/>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="inlineStr"/>
+      <c r="G284" t="inlineStr"/>
+      <c r="H284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>('LCA', 'Cement-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr"/>
+      <c r="D285" t="inlineStr"/>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="inlineStr"/>
+      <c r="G285" t="inlineStr"/>
+      <c r="H285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>('LCA', 'Concrete-H resources [points/m3]')</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr"/>
+      <c r="D286" t="inlineStr"/>
+      <c r="E286" t="inlineStr"/>
+      <c r="F286" t="inlineStr"/>
+      <c r="G286" t="inlineStr"/>
+      <c r="H286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>('LCA', 'Gravel-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+      <c r="G287" t="inlineStr"/>
+      <c r="H287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>('LCA', 'Plastic-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr"/>
+      <c r="D288" t="inlineStr"/>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="inlineStr"/>
+      <c r="G288" t="inlineStr"/>
+      <c r="H288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>('LCA', 'Sand-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr"/>
+      <c r="D289" t="inlineStr"/>
+      <c r="E289" t="inlineStr"/>
+      <c r="F289" t="inlineStr"/>
+      <c r="G289" t="inlineStr"/>
+      <c r="H289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>('LCA', 'Stainless steel-h resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr"/>
+      <c r="D290" t="inlineStr"/>
+      <c r="E290" t="inlineStr"/>
+      <c r="F290" t="inlineStr"/>
+      <c r="G290" t="inlineStr"/>
+      <c r="H290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>('LCA', 'Stainless steel sheet-h resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr"/>
+      <c r="D291" t="inlineStr"/>
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="inlineStr"/>
+      <c r="G291" t="inlineStr"/>
+      <c r="H291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>('LCA', 'Steel-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr"/>
+      <c r="D292" t="inlineStr"/>
+      <c r="E292" t="inlineStr"/>
+      <c r="F292" t="inlineStr"/>
+      <c r="G292" t="inlineStr"/>
+      <c r="H292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>('LCA', 'Wood-H resources [points/m3]')</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr"/>
+      <c r="D293" t="inlineStr"/>
+      <c r="E293" t="inlineStr"/>
+      <c r="F293" t="inlineStr"/>
+      <c r="G293" t="inlineStr"/>
+      <c r="H293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>('LCA', 'Trucking-H resources [points/tonne*km]')</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr"/>
+      <c r="D294" t="inlineStr"/>
+      <c r="E294" t="inlineStr"/>
+      <c r="F294" t="inlineStr"/>
+      <c r="G294" t="inlineStr"/>
+      <c r="H294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>('LCA', 'Metal-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr"/>
+      <c r="D295" t="inlineStr"/>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+      <c r="G295" t="inlineStr"/>
+      <c r="H295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>('LCA', 'Pump-H resources [points/ea]')</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr"/>
+      <c r="D296" t="inlineStr"/>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+      <c r="G296" t="inlineStr"/>
+      <c r="H296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>('LCA', 'Solar-H resources [points/m2]')</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr"/>
+      <c r="D297" t="inlineStr"/>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+      <c r="G297" t="inlineStr"/>
+      <c r="H297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>('LCA', 'Fan-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr"/>
+      <c r="D298" t="inlineStr"/>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+      <c r="G298" t="inlineStr"/>
+      <c r="H298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>('LCA', 'Battery-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr"/>
+      <c r="D299" t="inlineStr"/>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+      <c r="G299" t="inlineStr"/>
+      <c r="H299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>('LCA', 'Ceramic-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr"/>
+      <c r="D300" t="inlineStr"/>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+      <c r="G300" t="inlineStr"/>
+      <c r="H300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>('LCA', 'FRP-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="inlineStr"/>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+      <c r="G301" t="inlineStr"/>
+      <c r="H301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>('LCA', 'Na cl-h resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="inlineStr"/>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+      <c r="G302" t="inlineStr"/>
+      <c r="H302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>('LCA', 'Motor-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="inlineStr"/>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+      <c r="G303" t="inlineStr"/>
+      <c r="H303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>('LCA', 'Titanium-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+      <c r="G304" t="inlineStr"/>
+      <c r="H304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>('LCA', 'PVC-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+      <c r="G305" t="inlineStr"/>
+      <c r="H305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity CF [kg CO2-eq/kWh]')</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr"/>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+      <c r="G306" t="inlineStr"/>
+      <c r="H306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity ecosystems CF [points/kWh]')</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr"/>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+      <c r="G307" t="inlineStr"/>
+      <c r="H307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity health CF [points/kWh]')</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="inlineStr"/>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+      <c r="G308" t="inlineStr"/>
+      <c r="H308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity resources CF [points/kWh]')</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+      <c r="G309" t="inlineStr"/>
+      <c r="H309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>('TEA', 'Price factor [-]')</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr"/>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+      <c r="G310" t="inlineStr"/>
+      <c r="H310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>('TEA', 'N fertilizer price [USD/kg N]')</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+      <c r="G311" t="inlineStr"/>
+      <c r="H311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>('TEA', 'P fertilizer price [USD/kg P]')</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr"/>
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+      <c r="G312" t="inlineStr"/>
+      <c r="H312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>('TEA', 'K fertilizer price [USD/kg K]')</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr"/>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+      <c r="G313" t="inlineStr"/>
+      <c r="H313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>('TEA', 'NH3 fertilizer price [USD/kg N]')</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr"/>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+      <c r="G314" t="inlineStr"/>
+      <c r="H314" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4978,7 +5490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H294"/>
+  <dimension ref="A1:H326"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7717,7 +8229,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>('Ion exchange reclaimer-C6', 'TN removal [% removal ]')</t>
+          <t>('Ion exchange reclaimer-C6', 'TN removal [ratio]')</t>
         </is>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -7797,7 +8309,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>('Ion exchange reclaimer-C6', 'Desorption recovery efficiency [% recovery]')</t>
+          <t>('Ion exchange reclaimer-C6', 'Desorption recovery efficiency [ratio]')</t>
         </is>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -8101,7 +8613,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>('LCA', 'CH4 resources CF [points/kg CH4]')</t>
+          <t>('LCA', 'N2O CF [kg CO2-eq/kg N2O]')</t>
         </is>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -8117,7 +8629,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O CF [kg CO2-eq/kg N2O]')</t>
+          <t>('LCA', 'N2O ecosystems CF [points/kg N2O]')</t>
         </is>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -8133,7 +8645,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O ecosystems CF [points/kg N2O]')</t>
+          <t>('LCA', 'N2O health CF [points/kg N2O]')</t>
         </is>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -8149,7 +8661,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O health CF [points/kg N2O]')</t>
+          <t>('LCA', 'N fertilizer CF [kg CO2-eq/kg N]')</t>
         </is>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -8165,7 +8677,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>('LCA', 'N2O resources CF [points/kg N2O]')</t>
+          <t>('LCA', 'N fertilizer ecosystems CF [points/kg N]')</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
@@ -8181,7 +8693,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-Global warming [kg CO2-eq/m3]')</t>
+          <t>('LCA', 'N fertilizer health CF [points/kg N]')</t>
         </is>
       </c>
       <c r="C199" t="inlineStr"/>
@@ -8197,7 +8709,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'N fertilizer resources CF [points/kg N]')</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -8213,7 +8725,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'P fertilizer CF [kg CO2-eq/kg P]')</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -8229,7 +8741,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-Global warming [kg CO2-eq/m3]')</t>
+          <t>('LCA', 'P fertilizer ecosystems CF [points/kg P]')</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -8245,7 +8757,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'P fertilizer health CF [points/kg P]')</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -8261,7 +8773,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'P fertilizer resources CF [points/kg P]')</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -8277,7 +8789,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'K fertilizer CF [kg CO2-eq/kg K]')</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -8293,7 +8805,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Conc nh3 CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -8309,7 +8821,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Conc nh3 ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C207" t="inlineStr"/>
@@ -8325,7 +8837,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Conc nh3 health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C208" t="inlineStr"/>
@@ -8341,7 +8853,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-Global warming [kg CO2-eq/m3]')</t>
+          <t>('LCA', 'Conc nh3 resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -8357,7 +8869,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-Global warming [kg CO2-eq/tonne*km]')</t>
+          <t>('LCA', 'GAC CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -8373,7 +8885,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'GAC ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -8389,7 +8901,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-Global warming [kg CO2-eq/ea]')</t>
+          <t>('LCA', 'GAC health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -8405,7 +8917,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-Global warming [kg CO2-eq/m2]')</t>
+          <t>('LCA', 'GAC resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -8421,7 +8933,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -8437,7 +8949,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -8453,7 +8965,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C216" t="inlineStr"/>
@@ -8469,7 +8981,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'Zeolite resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C217" t="inlineStr"/>
@@ -8485,7 +8997,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -8501,7 +9013,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -8517,7 +9029,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -8533,7 +9045,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-Global warming [kg CO2-eq/kg]')</t>
+          <t>('LCA', 'KCl resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -8549,7 +9061,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-H ecosystems [points/m3]')</t>
+          <t>('LCA', 'Mg oh2 CF [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -8565,7 +9077,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Mg oh2 ecosystems CF [points/kg]')</t>
         </is>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -8581,7 +9093,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Mg oh2 health CF [points/kg]')</t>
         </is>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -8597,7 +9109,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-H ecosystems [points/m3]')</t>
+          <t>('LCA', 'Mg oh2 resources CF [points/kg]')</t>
         </is>
       </c>
       <c r="C225" t="inlineStr"/>
@@ -8613,7 +9125,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Excavation-Global warming [kg CO2-eq/m3]')</t>
         </is>
       </c>
       <c r="C226" t="inlineStr"/>
@@ -8629,7 +9141,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Brick-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -8645,7 +9157,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Cement-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C228" t="inlineStr"/>
@@ -8661,7 +9173,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-h ecosystems [points/kg]')</t>
+          <t>('LCA', 'Concrete-Global warming [kg CO2-eq/m3]')</t>
         </is>
       </c>
       <c r="C229" t="inlineStr"/>
@@ -8677,7 +9189,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-h ecosystems [points/kg]')</t>
+          <t>('LCA', 'Gravel-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C230" t="inlineStr"/>
@@ -8693,7 +9205,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Plastic-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C231" t="inlineStr"/>
@@ -8709,7 +9221,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-H ecosystems [points/m3]')</t>
+          <t>('LCA', 'Sand-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C232" t="inlineStr"/>
@@ -8725,7 +9237,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-H ecosystems [points/tonne*km]')</t>
+          <t>('LCA', 'Stainless steel-global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C233" t="inlineStr"/>
@@ -8741,7 +9253,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet-global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C234" t="inlineStr"/>
@@ -8757,7 +9269,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-H ecosystems [points/ea]')</t>
+          <t>('LCA', 'Steel-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C235" t="inlineStr"/>
@@ -8773,7 +9285,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-H ecosystems [points/m2]')</t>
+          <t>('LCA', 'Wood-Global warming [kg CO2-eq/m3]')</t>
         </is>
       </c>
       <c r="C236" t="inlineStr"/>
@@ -8789,7 +9301,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Trucking-Global warming [kg CO2-eq/tonne*km]')</t>
         </is>
       </c>
       <c r="C237" t="inlineStr"/>
@@ -8805,7 +9317,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Metal-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C238" t="inlineStr"/>
@@ -8821,7 +9333,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Pump-Global warming [kg CO2-eq/ea]')</t>
         </is>
       </c>
       <c r="C239" t="inlineStr"/>
@@ -8837,7 +9349,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Solar-Global warming [kg CO2-eq/m2]')</t>
         </is>
       </c>
       <c r="C240" t="inlineStr"/>
@@ -8853,7 +9365,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-h ecosystems [points/kg]')</t>
+          <t>('LCA', 'Fan-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C241" t="inlineStr"/>
@@ -8869,7 +9381,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Battery-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C242" t="inlineStr"/>
@@ -8885,7 +9397,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'Ceramic-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C243" t="inlineStr"/>
@@ -8901,7 +9413,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-H ecosystems [points/kg]')</t>
+          <t>('LCA', 'FRP-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C244" t="inlineStr"/>
@@ -8917,7 +9429,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-H health [points/m3]')</t>
+          <t>('LCA', 'Na cl-global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C245" t="inlineStr"/>
@@ -8933,7 +9445,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-H health [points/kg]')</t>
+          <t>('LCA', 'Motor-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C246" t="inlineStr"/>
@@ -8949,7 +9461,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-H health [points/kg]')</t>
+          <t>('LCA', 'Titanium-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C247" t="inlineStr"/>
@@ -8965,7 +9477,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-H health [points/m3]')</t>
+          <t>('LCA', 'PVC-Global warming [kg CO2-eq/kg]')</t>
         </is>
       </c>
       <c r="C248" t="inlineStr"/>
@@ -8981,7 +9493,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-H health [points/kg]')</t>
+          <t>('LCA', 'Excavation-H ecosystems [points/m3]')</t>
         </is>
       </c>
       <c r="C249" t="inlineStr"/>
@@ -8997,7 +9509,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-H health [points/kg]')</t>
+          <t>('LCA', 'Brick-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C250" t="inlineStr"/>
@@ -9013,7 +9525,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-H health [points/kg]')</t>
+          <t>('LCA', 'Cement-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C251" t="inlineStr"/>
@@ -9029,7 +9541,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-h health [points/kg]')</t>
+          <t>('LCA', 'Concrete-H ecosystems [points/m3]')</t>
         </is>
       </c>
       <c r="C252" t="inlineStr"/>
@@ -9045,7 +9557,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-h health [points/kg]')</t>
+          <t>('LCA', 'Gravel-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C253" t="inlineStr"/>
@@ -9061,7 +9573,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-H health [points/kg]')</t>
+          <t>('LCA', 'Plastic-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C254" t="inlineStr"/>
@@ -9077,7 +9589,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-H health [points/m3]')</t>
+          <t>('LCA', 'Sand-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C255" t="inlineStr"/>
@@ -9093,7 +9605,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-H health [points/tonne*km]')</t>
+          <t>('LCA', 'Stainless steel-h ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C256" t="inlineStr"/>
@@ -9109,7 +9621,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-H health [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet-h ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C257" t="inlineStr"/>
@@ -9125,7 +9637,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-H health [points/ea]')</t>
+          <t>('LCA', 'Steel-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C258" t="inlineStr"/>
@@ -9141,7 +9653,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-H health [points/m2]')</t>
+          <t>('LCA', 'Wood-H ecosystems [points/m3]')</t>
         </is>
       </c>
       <c r="C259" t="inlineStr"/>
@@ -9157,7 +9669,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-H health [points/kg]')</t>
+          <t>('LCA', 'Trucking-H ecosystems [points/tonne*km]')</t>
         </is>
       </c>
       <c r="C260" t="inlineStr"/>
@@ -9173,7 +9685,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-H health [points/kg]')</t>
+          <t>('LCA', 'Metal-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C261" t="inlineStr"/>
@@ -9189,7 +9701,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-H health [points/kg]')</t>
+          <t>('LCA', 'Pump-H ecosystems [points/ea]')</t>
         </is>
       </c>
       <c r="C262" t="inlineStr"/>
@@ -9205,7 +9717,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-H health [points/kg]')</t>
+          <t>('LCA', 'Solar-H ecosystems [points/m2]')</t>
         </is>
       </c>
       <c r="C263" t="inlineStr"/>
@@ -9221,7 +9733,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-h health [points/kg]')</t>
+          <t>('LCA', 'Fan-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C264" t="inlineStr"/>
@@ -9237,7 +9749,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-H health [points/kg]')</t>
+          <t>('LCA', 'Battery-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C265" t="inlineStr"/>
@@ -9253,7 +9765,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-H health [points/kg]')</t>
+          <t>('LCA', 'Ceramic-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C266" t="inlineStr"/>
@@ -9269,7 +9781,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-H health [points/kg]')</t>
+          <t>('LCA', 'FRP-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C267" t="inlineStr"/>
@@ -9285,7 +9797,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation-H resources [points/m3]')</t>
+          <t>('LCA', 'Na cl-h ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C268" t="inlineStr"/>
@@ -9301,7 +9813,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick-H resources [points/kg]')</t>
+          <t>('LCA', 'Motor-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C269" t="inlineStr"/>
@@ -9317,7 +9829,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement-H resources [points/kg]')</t>
+          <t>('LCA', 'Titanium-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C270" t="inlineStr"/>
@@ -9333,7 +9845,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete-H resources [points/m3]')</t>
+          <t>('LCA', 'PVC-H ecosystems [points/kg]')</t>
         </is>
       </c>
       <c r="C271" t="inlineStr"/>
@@ -9349,7 +9861,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel-H resources [points/kg]')</t>
+          <t>('LCA', 'Excavation-H health [points/m3]')</t>
         </is>
       </c>
       <c r="C272" t="inlineStr"/>
@@ -9365,7 +9877,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic-H resources [points/kg]')</t>
+          <t>('LCA', 'Brick-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C273" t="inlineStr"/>
@@ -9381,7 +9893,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand-H resources [points/kg]')</t>
+          <t>('LCA', 'Cement-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C274" t="inlineStr"/>
@@ -9397,7 +9909,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel-h resources [points/kg]')</t>
+          <t>('LCA', 'Concrete-H health [points/m3]')</t>
         </is>
       </c>
       <c r="C275" t="inlineStr"/>
@@ -9413,7 +9925,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet-h resources [points/kg]')</t>
+          <t>('LCA', 'Gravel-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C276" t="inlineStr"/>
@@ -9429,7 +9941,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel-H resources [points/kg]')</t>
+          <t>('LCA', 'Plastic-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C277" t="inlineStr"/>
@@ -9445,7 +9957,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood-H resources [points/m3]')</t>
+          <t>('LCA', 'Sand-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C278" t="inlineStr"/>
@@ -9461,7 +9973,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking-H resources [points/tonne*km]')</t>
+          <t>('LCA', 'Stainless steel-h health [points/kg]')</t>
         </is>
       </c>
       <c r="C279" t="inlineStr"/>
@@ -9477,7 +9989,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>('LCA', 'Metal-H resources [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet-h health [points/kg]')</t>
         </is>
       </c>
       <c r="C280" t="inlineStr"/>
@@ -9493,7 +10005,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>('LCA', 'Pump-H resources [points/ea]')</t>
+          <t>('LCA', 'Steel-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C281" t="inlineStr"/>
@@ -9509,7 +10021,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>('LCA', 'Solar-H resources [points/m2]')</t>
+          <t>('LCA', 'Wood-H health [points/m3]')</t>
         </is>
       </c>
       <c r="C282" t="inlineStr"/>
@@ -9525,7 +10037,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>('LCA', 'Fan-H resources [points/kg]')</t>
+          <t>('LCA', 'Trucking-H health [points/tonne*km]')</t>
         </is>
       </c>
       <c r="C283" t="inlineStr"/>
@@ -9541,7 +10053,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>('LCA', 'Battery-H resources [points/kg]')</t>
+          <t>('LCA', 'Metal-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C284" t="inlineStr"/>
@@ -9557,7 +10069,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>('LCA', 'Ceramic-H resources [points/kg]')</t>
+          <t>('LCA', 'Pump-H health [points/ea]')</t>
         </is>
       </c>
       <c r="C285" t="inlineStr"/>
@@ -9573,7 +10085,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>('LCA', 'FRP-H resources [points/kg]')</t>
+          <t>('LCA', 'Solar-H health [points/m2]')</t>
         </is>
       </c>
       <c r="C286" t="inlineStr"/>
@@ -9589,7 +10101,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>('LCA', 'Na cl-h resources [points/kg]')</t>
+          <t>('LCA', 'Fan-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C287" t="inlineStr"/>
@@ -9605,7 +10117,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>('LCA', 'Motor-H resources [points/kg]')</t>
+          <t>('LCA', 'Battery-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C288" t="inlineStr"/>
@@ -9621,7 +10133,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>('LCA', 'Titanium-H resources [points/kg]')</t>
+          <t>('LCA', 'Ceramic-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C289" t="inlineStr"/>
@@ -9637,7 +10149,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>('LCA', 'PVC-H resources [points/kg]')</t>
+          <t>('LCA', 'FRP-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C290" t="inlineStr"/>
@@ -9653,7 +10165,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity CF [kg CO2-eq/kWh]')</t>
+          <t>('LCA', 'Na cl-h health [points/kg]')</t>
         </is>
       </c>
       <c r="C291" t="inlineStr"/>
@@ -9669,7 +10181,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity ecosystems CF [points/kWh]')</t>
+          <t>('LCA', 'Motor-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C292" t="inlineStr"/>
@@ -9685,7 +10197,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity health CF [points/kWh]')</t>
+          <t>('LCA', 'Titanium-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C293" t="inlineStr"/>
@@ -9701,7 +10213,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>('LCA', 'Electricity resources CF [points/kWh]')</t>
+          <t>('LCA', 'PVC-H health [points/kg]')</t>
         </is>
       </c>
       <c r="C294" t="inlineStr"/>
@@ -9711,6 +10223,518 @@
       <c r="G294" t="inlineStr"/>
       <c r="H294" t="inlineStr"/>
     </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>('LCA', 'Excavation-H resources [points/m3]')</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr"/>
+      <c r="D295" t="inlineStr"/>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+      <c r="G295" t="inlineStr"/>
+      <c r="H295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>('LCA', 'Brick-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr"/>
+      <c r="D296" t="inlineStr"/>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+      <c r="G296" t="inlineStr"/>
+      <c r="H296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>('LCA', 'Cement-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr"/>
+      <c r="D297" t="inlineStr"/>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+      <c r="G297" t="inlineStr"/>
+      <c r="H297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>('LCA', 'Concrete-H resources [points/m3]')</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr"/>
+      <c r="D298" t="inlineStr"/>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+      <c r="G298" t="inlineStr"/>
+      <c r="H298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>('LCA', 'Gravel-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr"/>
+      <c r="D299" t="inlineStr"/>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+      <c r="G299" t="inlineStr"/>
+      <c r="H299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>('LCA', 'Plastic-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr"/>
+      <c r="D300" t="inlineStr"/>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+      <c r="G300" t="inlineStr"/>
+      <c r="H300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>('LCA', 'Sand-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="inlineStr"/>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+      <c r="G301" t="inlineStr"/>
+      <c r="H301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>('LCA', 'Stainless steel-h resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="inlineStr"/>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+      <c r="G302" t="inlineStr"/>
+      <c r="H302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>('LCA', 'Stainless steel sheet-h resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="inlineStr"/>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+      <c r="G303" t="inlineStr"/>
+      <c r="H303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>('LCA', 'Steel-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+      <c r="G304" t="inlineStr"/>
+      <c r="H304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>('LCA', 'Wood-H resources [points/m3]')</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+      <c r="G305" t="inlineStr"/>
+      <c r="H305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>('LCA', 'Trucking-H resources [points/tonne*km]')</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr"/>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+      <c r="G306" t="inlineStr"/>
+      <c r="H306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>('LCA', 'Metal-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr"/>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+      <c r="G307" t="inlineStr"/>
+      <c r="H307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>('LCA', 'Pump-H resources [points/ea]')</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="inlineStr"/>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+      <c r="G308" t="inlineStr"/>
+      <c r="H308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>('LCA', 'Solar-H resources [points/m2]')</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+      <c r="G309" t="inlineStr"/>
+      <c r="H309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>('LCA', 'Fan-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr"/>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+      <c r="G310" t="inlineStr"/>
+      <c r="H310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>('LCA', 'Battery-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+      <c r="G311" t="inlineStr"/>
+      <c r="H311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>('LCA', 'Ceramic-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr"/>
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+      <c r="G312" t="inlineStr"/>
+      <c r="H312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>('LCA', 'FRP-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr"/>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+      <c r="G313" t="inlineStr"/>
+      <c r="H313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>('LCA', 'Na cl-h resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr"/>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+      <c r="G314" t="inlineStr"/>
+      <c r="H314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>('LCA', 'Motor-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="inlineStr"/>
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+      <c r="G315" t="inlineStr"/>
+      <c r="H315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>('LCA', 'Titanium-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr"/>
+      <c r="D316" t="inlineStr"/>
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+      <c r="G316" t="inlineStr"/>
+      <c r="H316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>('LCA', 'PVC-H resources [points/kg]')</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="inlineStr"/>
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+      <c r="G317" t="inlineStr"/>
+      <c r="H317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity CF [kg CO2-eq/kWh]')</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="inlineStr"/>
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="inlineStr"/>
+      <c r="G318" t="inlineStr"/>
+      <c r="H318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity ecosystems CF [points/kWh]')</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="inlineStr"/>
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+      <c r="G319" t="inlineStr"/>
+      <c r="H319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity health CF [points/kWh]')</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr"/>
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+      <c r="G320" t="inlineStr"/>
+      <c r="H320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>('LCA', 'Electricity resources CF [points/kWh]')</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="inlineStr"/>
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+      <c r="G321" t="inlineStr"/>
+      <c r="H321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>('TEA', 'Price factor [-]')</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="inlineStr"/>
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+      <c r="G322" t="inlineStr"/>
+      <c r="H322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>('TEA', 'N fertilizer price [USD/kg N]')</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr"/>
+      <c r="D323" t="inlineStr"/>
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="inlineStr"/>
+      <c r="G323" t="inlineStr"/>
+      <c r="H323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>('TEA', 'P fertilizer price [USD/kg P]')</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="inlineStr"/>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="inlineStr"/>
+      <c r="G324" t="inlineStr"/>
+      <c r="H324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>('TEA', 'K fertilizer price [USD/kg K]')</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="inlineStr"/>
+      <c r="E325" t="inlineStr"/>
+      <c r="F325" t="inlineStr"/>
+      <c r="G325" t="inlineStr"/>
+      <c r="H325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>('TEA', 'NH3 fertilizer price [USD/kg N]')</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr"/>
+      <c r="D326" t="inlineStr"/>
+      <c r="E326" t="inlineStr"/>
+      <c r="F326" t="inlineStr"/>
+      <c r="G326" t="inlineStr"/>
+      <c r="H326" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>